<commit_message>
Updates to plans based on our meeting
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan11332\Development\Top 20 Python\Proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan11332\Development\Top 20 Python\Top-20-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2954DA6A-CDB4-46E4-B109-96969A5C0D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4B757D-AA57-44B4-803E-1863A48B3664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="30" windowWidth="38640" windowHeight="21120" xr2:uid="{489E7116-D3BD-4C32-AB15-5D899FD5D120}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{489E7116-D3BD-4C32-AB15-5D899FD5D120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Preface</t>
   </si>
@@ -50,15 +50,9 @@
     <t>Chapter 2</t>
   </si>
   <si>
-    <t>Functional Programming – ArcPy Basics</t>
-  </si>
-  <si>
     <t>Chapter 3</t>
   </si>
   <si>
-    <t>Functional Programming – ArcGIS Python API Basics</t>
-  </si>
-  <si>
     <t>Chapter 4</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>Chapter 8</t>
   </si>
   <si>
-    <t>AI / ML</t>
-  </si>
-  <si>
     <t>Chapter 9</t>
   </si>
   <si>
@@ -158,9 +149,6 @@
     <t>Chapter 20</t>
   </si>
   <si>
-    <t>Continuing your Python Journey</t>
-  </si>
-  <si>
     <t>Chapter</t>
   </si>
   <si>
@@ -176,13 +164,31 @@
     <t>Dan</t>
   </si>
   <si>
-    <t>Intro</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
     <t>Chapters</t>
+  </si>
+  <si>
+    <t>Intro (Setup, Pythonic Principles, etc)</t>
+  </si>
+  <si>
+    <t>ArcPy Basics</t>
+  </si>
+  <si>
+    <t>ArcGIS Python API Basics</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Parallel Processing (after data engineering)</t>
+  </si>
+  <si>
+    <t>Data Processing</t>
+  </si>
+  <si>
+    <t>Parellel processing</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -235,15 +241,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -254,6 +280,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E88BDB1-727B-4884-8716-647E6604F4C5}" name="Table1" displayName="Table1" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22" xr:uid="{3E88BDB1-727B-4884-8716-647E6604F4C5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C22">
+    <sortCondition ref="C1:C22"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A130BE25-6103-434A-AC2B-70A6CF4A9946}" name="Chapter" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{29983084-FB65-4B71-8CD9-64BDACF13FB0}" name="Title" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{48197A1C-A14B-45BA-A37E-78E972ED5AB9}" name="Author"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -553,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6117777E-3B8B-469C-AC0A-4ACE1E7A92D2}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,280 +607,295 @@
     <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
       <c r="G4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F5">
         <f>COUNTIF(C:C,E5)</f>
         <v>11</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f>(250/21)*F5</f>
         <v>130.95238095238096</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <f>COUNTIF(C:C,E6)</f>
         <v>10</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f>(250/21)*F6</f>
         <v>119.04761904761905</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>